<commit_message>
y2s1: Week 15 Release 0.1
</commit_message>
<xml_diff>
--- a/y2s1/statistics-ii/tutorials/stat2t7.xlsx
+++ b/y2s1/statistics-ii/tutorials/stat2t7.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user300\repo\dco-1820\y2s1\statistics-ii\tutorials\excel-tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user300\repo\dco-1820\y2s1\statistics-ii\tutorials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9FFC7D-0FBA-485E-BDF0-9CD38910C213}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB681D66-4F1D-4772-8598-976F35B2D1C4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14340" yWindow="3040" windowWidth="14400" windowHeight="7440" activeTab="1" xr2:uid="{E804A53E-73EF-40F2-B56C-269591973950}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="15375" windowHeight="7815" firstSheet="1" activeTab="2" xr2:uid="{E804A53E-73EF-40F2-B56C-269591973950}"/>
   </bookViews>
   <sheets>
     <sheet name="Tutorial 7" sheetId="1" r:id="rId1"/>
     <sheet name="Practice Materials" sheetId="2" r:id="rId2"/>
+    <sheet name="Practice x2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="68">
   <si>
     <t>Intensity of bookings</t>
   </si>
@@ -296,13 +297,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,24 +620,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B06475EA-05AC-4DDE-923F-B0F31A1DEA38}">
   <dimension ref="A1:J96"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94:C96"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.81640625" customWidth="1"/>
-    <col min="2" max="2" width="15.1796875" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" customWidth="1"/>
-    <col min="4" max="5" width="15.26953125" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="5" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -659,7 +660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -686,36 +687,36 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>47</v>
       </c>
       <c r="B5">
-        <f>1/6</f>
+        <f t="shared" ref="B5:G5" si="0">1/6</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="C5">
-        <f>1/6</f>
+        <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="D5">
-        <f>1/6</f>
+        <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="E5">
-        <f>1/6</f>
+        <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="F5">
-        <f>1/6</f>
+        <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="G5">
-        <f>1/6</f>
+        <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -724,27 +725,27 @@
         <v>22</v>
       </c>
       <c r="C6">
-        <f t="shared" ref="C6:G6" si="0">C5*132</f>
+        <f t="shared" ref="C6:G6" si="1">C5*132</f>
         <v>22</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -753,23 +754,23 @@
         <v>1.6363636363636365</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:G7" si="1">(C4-C6)^2/C6</f>
+        <f t="shared" ref="C7:G7" si="2">(C4-C6)^2/C6</f>
         <v>0.18181818181818182</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.40909090909090912</v>
       </c>
       <c r="E7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9090909090909092</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.2272727272727271</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6363636363636365</v>
       </c>
       <c r="H7">
@@ -777,15 +778,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -814,7 +815,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -847,7 +848,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -884,7 +885,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -893,44 +894,44 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:I14" si="2">(C12-C13)^2/C13</f>
+        <f t="shared" ref="C14:I14" si="3">(C12-C13)^2/C13</f>
         <v>0.125</v>
       </c>
       <c r="D14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.125</v>
       </c>
       <c r="F14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="G14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="I14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="5">
         <f>SUM(B14:I14)</f>
         <v>2.25</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -953,7 +954,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -980,7 +981,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -1003,7 +1004,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1012,23 +1013,23 @@
         <v>111</v>
       </c>
       <c r="C21">
-        <f t="shared" ref="C21:G21" si="3">C20*370</f>
+        <f t="shared" ref="C21:G21" si="4">C20*370</f>
         <v>74</v>
       </c>
       <c r="D21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>74</v>
       </c>
       <c r="E21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
       <c r="F21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
       <c r="G21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
       <c r="H21">
@@ -1036,7 +1037,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1045,23 +1046,23 @@
         <v>6.5675675675675675</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:H22" si="4">(C19-C21)^2/C21</f>
+        <f t="shared" ref="C22:G22" si="5">(C19-C21)^2/C21</f>
         <v>0.33783783783783783</v>
       </c>
       <c r="D22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.3513513513513514E-2</v>
       </c>
       <c r="E22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.8918918918918921</v>
       </c>
       <c r="F22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.7027027027027029E-2</v>
       </c>
       <c r="G22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.7027027027027026</v>
       </c>
       <c r="H22">
@@ -1069,12 +1070,12 @@
         <v>13.54054054054054</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="7" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -1088,7 +1089,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1106,7 +1107,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -1120,7 +1121,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1129,15 +1130,15 @@
         <v>30</v>
       </c>
       <c r="C29">
-        <f t="shared" ref="C29:D29" si="5">C28*100</f>
+        <f t="shared" ref="C29:D29" si="6">C28*100</f>
         <v>40</v>
       </c>
       <c r="D29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1146,11 +1147,11 @@
         <v>1.2</v>
       </c>
       <c r="C30">
-        <f t="shared" ref="C30:D30" si="6">(C27-C29)^2/C29</f>
+        <f t="shared" ref="C30:D30" si="7">(C27-C29)^2/C29</f>
         <v>0.22500000000000001</v>
       </c>
       <c r="D30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.7</v>
       </c>
       <c r="E30">
@@ -1158,8 +1159,8 @@
         <v>4.125</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="7" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B32" t="s">
@@ -1181,7 +1182,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>46</v>
       </c>
@@ -1205,7 +1206,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>47</v>
       </c>
@@ -1214,23 +1215,23 @@
         <v>6.25E-2</v>
       </c>
       <c r="D34">
-        <f t="shared" ref="D34:G34" si="7">_xlfn.BINOM.DIST(D32,4,0.5,)</f>
+        <f t="shared" ref="D34:G34" si="8">_xlfn.BINOM.DIST(D32,4,0.5,)</f>
         <v>0.24999999999999994</v>
       </c>
       <c r="E34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.375</v>
       </c>
       <c r="F34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.25</v>
       </c>
       <c r="G34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>30</v>
       </c>
@@ -1239,23 +1240,23 @@
         <v>6.25</v>
       </c>
       <c r="D35">
-        <f t="shared" ref="D35:G35" si="8">D34*100</f>
+        <f t="shared" ref="D35:G35" si="9">D34*100</f>
         <v>24.999999999999993</v>
       </c>
       <c r="E35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>37.5</v>
       </c>
       <c r="F35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>25</v>
       </c>
       <c r="G35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.25</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>31</v>
       </c>
@@ -1264,44 +1265,44 @@
         <v>0.25</v>
       </c>
       <c r="D36">
-        <f t="shared" ref="D36:G36" si="9">(D33-D35)^2/D35</f>
+        <f t="shared" ref="D36:G36" si="10">(D33-D35)^2/D35</f>
         <v>0.15999999999999892</v>
       </c>
       <c r="E36">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.06</v>
       </c>
       <c r="F36">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.44</v>
       </c>
       <c r="G36">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>9.61</v>
       </c>
-      <c r="H36" s="7">
+      <c r="H36" s="5">
         <f>SUM(C36:G36)</f>
         <v>11.519999999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="5" t="s">
+    <row r="40" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" s="5"/>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
       <c r="B41" t="s">
         <v>2</v>
       </c>
@@ -1315,7 +1316,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -1333,7 +1334,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -1351,7 +1352,7 @@
       </c>
       <c r="E43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -1369,7 +1370,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -1387,7 +1388,7 @@
       </c>
       <c r="E45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -1408,24 +1409,24 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" s="5" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="5"/>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
       <c r="B50" t="s">
         <v>19</v>
       </c>
@@ -1439,7 +1440,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>23</v>
       </c>
@@ -1457,7 +1458,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -1475,7 +1476,7 @@
       </c>
       <c r="E52" s="2"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>24</v>
       </c>
@@ -1493,7 +1494,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -1511,7 +1512,7 @@
       </c>
       <c r="E54" s="2"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>25</v>
       </c>
@@ -1529,7 +1530,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -1547,7 +1548,7 @@
       </c>
       <c r="E56" s="2"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>8</v>
       </c>
@@ -1556,11 +1557,11 @@
         <v>60</v>
       </c>
       <c r="C57">
-        <f t="shared" ref="C57:D57" si="10">C51+C53+C55</f>
+        <f t="shared" ref="C57:D57" si="11">C51+C53+C55</f>
         <v>240</v>
       </c>
       <c r="D57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>300</v>
       </c>
       <c r="F57">
@@ -1568,25 +1569,25 @@
         <v>600</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61" s="5" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B61" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C61" s="6"/>
-      <c r="D61" s="6"/>
-      <c r="E61" s="6"/>
-      <c r="F61" s="6"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="5"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="6"/>
       <c r="B62" t="s">
         <v>12</v>
       </c>
@@ -1603,7 +1604,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>16</v>
       </c>
@@ -1624,7 +1625,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>7</v>
       </c>
@@ -1645,7 +1646,7 @@
         <v>19.722222222222221</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>28</v>
       </c>
@@ -1666,7 +1667,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>7</v>
       </c>
@@ -1687,7 +1688,7 @@
         <v>20.416666666666668</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>17</v>
       </c>
@@ -1708,7 +1709,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -1729,7 +1730,7 @@
         <v>9.8611111111111107</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>8</v>
       </c>
@@ -1746,7 +1747,7 @@
         <v>140</v>
       </c>
       <c r="E69">
-        <f t="shared" ref="E69" si="11">E63+E65+E67</f>
+        <f t="shared" ref="E69" si="12">E63+E65+E67</f>
         <v>50</v>
       </c>
       <c r="F69">
@@ -1754,7 +1755,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>29</v>
       </c>
@@ -1765,7 +1766,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <f>B63</f>
         <v>26</v>
@@ -1779,7 +1780,7 @@
         <v>9.4008495416946086E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <f>C63</f>
         <v>43</v>
@@ -1789,11 +1790,11 @@
         <v>39.444444444444443</v>
       </c>
       <c r="C73" s="3">
-        <f t="shared" ref="C73:C83" si="12">(A73-B73)^2/B73</f>
+        <f t="shared" ref="C73:C83" si="13">(A73-B73)^2/B73</f>
         <v>0.32050078247261377</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <f>D63</f>
         <v>62</v>
@@ -1803,11 +1804,11 @@
         <v>55.222222222222221</v>
       </c>
       <c r="C74" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.83188016990833913</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <f>E63</f>
         <v>11</v>
@@ -1817,11 +1818,11 @@
         <v>19.722222222222221</v>
       </c>
       <c r="C75" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.8574334898278555</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <f>B65</f>
         <v>28</v>
@@ -1831,11 +1832,11 @@
         <v>28.583333333333332</v>
       </c>
       <c r="C76" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.1904761904761857E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <f>C65</f>
         <v>40</v>
@@ -1845,11 +1846,11 @@
         <v>40.833333333333336</v>
       </c>
       <c r="C77" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.7006802721088531E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <f>D65</f>
         <v>59</v>
@@ -1859,11 +1860,11 @@
         <v>57.166666666666664</v>
       </c>
       <c r="C78" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5.8794946550048743E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <f>E65</f>
         <v>20</v>
@@ -1873,11 +1874,11 @@
         <v>20.416666666666668</v>
       </c>
       <c r="C79" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>8.5034013605442653E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <f>B67</f>
         <v>16</v>
@@ -1887,11 +1888,11 @@
         <v>13.805555555555555</v>
       </c>
       <c r="C80" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.34881511289961997</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <f>C67</f>
         <v>17</v>
@@ -1901,11 +1902,11 @@
         <v>19.722222222222221</v>
       </c>
       <c r="C81" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.37574334898278539</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <f>D67</f>
         <v>19</v>
@@ -1915,11 +1916,11 @@
         <v>27.611111111111111</v>
       </c>
       <c r="C82" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.6855577911915938</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <f>E67</f>
         <v>19</v>
@@ -1929,11 +1930,11 @@
         <v>9.8611111111111107</v>
       </c>
       <c r="C83" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>8.4695618153364638</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="3" t="s">
         <v>32</v>
@@ -1943,12 +1944,12 @@
         <v>17.079710918572658</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>34</v>
       </c>
@@ -1962,7 +1963,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>37</v>
       </c>
@@ -1977,7 +1978,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>7</v>
       </c>
@@ -1991,12 +1992,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>38</v>
       </c>
@@ -2007,7 +2008,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>39</v>
       </c>
@@ -2022,7 +2023,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>41</v>
       </c>
@@ -2055,16 +2056,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA040C73-D898-4B5C-AE7A-712AD1E977BF}">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>3</v>
       </c>
@@ -2072,7 +2073,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -2095,7 +2096,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -2122,7 +2123,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -2155,14 +2156,14 @@
         <v>12.824999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B6" s="7">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="5">
         <v>250</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="5">
         <v>500</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <v>1000</v>
       </c>
       <c r="E6">
@@ -2172,18 +2173,18 @@
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
       <c r="B9" t="s">
         <v>19</v>
       </c>
@@ -2194,7 +2195,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -2215,7 +2216,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -2232,7 +2233,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -2253,7 +2254,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -2270,7 +2271,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -2291,7 +2292,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -2308,7 +2309,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -2332,7 +2333,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -2349,7 +2350,7 @@
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <f>(B12-B13)^2/B13</f>
         <v>0.41884057971014454</v>
@@ -2363,7 +2364,7 @@
         <v>0.18115942028985507</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22">
         <f>(B14-B15)^2/B15</f>
         <v>2.4888888888888885</v>
@@ -2376,25 +2377,25 @@
         <f t="shared" si="2"/>
         <v>1.0158730158730158</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="5">
         <f>SUM(B18:D22)</f>
         <v>9.0905012861534615</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="5" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="5"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
       <c r="B25" t="s">
         <v>12</v>
       </c>
@@ -2411,7 +2412,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -2432,7 +2433,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -2453,7 +2454,7 @@
         <v>19.722222222222221</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2474,7 +2475,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -2495,7 +2496,7 @@
         <v>20.416666666666668</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -2516,7 +2517,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -2537,7 +2538,7 @@
         <v>9.8611111111111107</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -2562,7 +2563,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -2583,7 +2584,7 @@
         <v>3.8574334898278555</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36">
         <f>(B28-B29)^2/B29</f>
         <v>1.1904761904761857E-2</v>
@@ -2601,7 +2602,7 @@
         <v>8.5034013605442653E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38">
         <f>(B30-B31)^2/B31</f>
         <v>0.34881511289961997</v>
@@ -2623,7 +2624,7 @@
         <v>17.079710918572658</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -2637,7 +2638,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>37</v>
       </c>
@@ -2652,7 +2653,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -2666,7 +2667,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>67</v>
       </c>
@@ -2683,7 +2684,7 @@
         <v>8.2810000000000006</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>38</v>
       </c>
@@ -2694,7 +2695,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -2709,7 +2710,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>30</v>
       </c>
@@ -2722,7 +2723,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>41</v>
       </c>
@@ -2737,7 +2738,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>30</v>
       </c>
@@ -2750,7 +2751,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51">
         <f>B47+B49</f>
         <v>140</v>
@@ -2764,7 +2765,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>67</v>
       </c>
@@ -2777,7 +2778,7 @@
         <v>0.67500000000000004</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55">
         <f>(ABS(B49-B50)-0.5)^2/B50</f>
         <v>0.28928571428571431</v>
@@ -2800,4 +2801,324 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6269139B-0747-4370-9E90-0B08ADC8D579}">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>29</v>
+      </c>
+      <c r="H3">
+        <v>28</v>
+      </c>
+      <c r="I3">
+        <f>SUM(C3:H3)</f>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <f>1/6*132</f>
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:H4" si="0">1/6*132</f>
+        <v>22</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5">
+        <f>(C3-C4)^2/C4</f>
+        <v>1.6363636363636365</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:H5" si="1">(D3-D4)^2/D4</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>2.9090909090909092</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>2.2272727272727271</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>1.6363636363636365</v>
+      </c>
+      <c r="I5">
+        <f>SUM(C5:H5)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>9</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>8</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <f>SUM(C8:J8)</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10">
+        <f>(C8-C9)^2/C9</f>
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="D10:J10" si="2">(D8-D9)^2/D9</f>
+        <v>0.125</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="K10">
+        <f>SUM(C10:J10)</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13">
+        <v>84</v>
+      </c>
+      <c r="D13">
+        <v>79</v>
+      </c>
+      <c r="E13">
+        <v>75</v>
+      </c>
+      <c r="F13">
+        <v>49</v>
+      </c>
+      <c r="G13">
+        <v>36</v>
+      </c>
+      <c r="H13">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
y2s1: Week 16 Release 0.1
</commit_message>
<xml_diff>
--- a/y2s1/statistics-ii/tutorials/stat2t7.xlsx
+++ b/y2s1/statistics-ii/tutorials/stat2t7.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user300\repo\dco-1820\y2s1\statistics-ii\tutorials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB681D66-4F1D-4772-8598-976F35B2D1C4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2325E8FE-E8B7-42B8-9D91-0DC1FB60972D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="15375" windowHeight="7815" firstSheet="1" activeTab="2" xr2:uid="{E804A53E-73EF-40F2-B56C-269591973950}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{E804A53E-73EF-40F2-B56C-269591973950}"/>
   </bookViews>
   <sheets>
     <sheet name="Tutorial 7" sheetId="1" r:id="rId1"/>
-    <sheet name="Practice Materials" sheetId="2" r:id="rId2"/>
-    <sheet name="Practice x2" sheetId="3" r:id="rId3"/>
+    <sheet name="Practice x2" sheetId="3" r:id="rId2"/>
+    <sheet name="Practice Materials" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="81">
   <si>
     <t>Intensity of bookings</t>
   </si>
@@ -237,6 +237,45 @@
   </si>
   <si>
     <t>(|Oi-Ei|-0.5)^2/Ei</t>
+  </si>
+  <si>
+    <t>Expected Proport</t>
+  </si>
+  <si>
+    <t>Screen size</t>
+  </si>
+  <si>
+    <t>Expected Proportion</t>
+  </si>
+  <si>
+    <t>Note: If all 4 coins are fair, then they should follow a binomial distribution with B(0.5,4)</t>
+  </si>
+  <si>
+    <t>Coin</t>
+  </si>
+  <si>
+    <t>Recovery</t>
+  </si>
+  <si>
+    <t>Group A</t>
+  </si>
+  <si>
+    <t>Group B</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>d &lt;= 1, Oi</t>
+  </si>
+  <si>
+    <t>1 &lt; d &lt; 2, Oi</t>
+  </si>
+  <si>
+    <t>d &gt;= 2, Oi</t>
+  </si>
+  <si>
+    <t>Chi-Square</t>
   </si>
 </sst>
 </file>
@@ -289,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -298,6 +337,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -620,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B06475EA-05AC-4DDE-923F-B0F31A1DEA38}">
   <dimension ref="A1:J96"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:G19"/>
+    <sheetView topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,18 +1333,18 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
       <c r="E40" s="1"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
+      <c r="A41" s="7"/>
       <c r="B41" t="s">
         <v>2</v>
       </c>
@@ -1415,18 +1457,18 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
       <c r="E49" s="1"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
+      <c r="A50" s="7"/>
       <c r="B50" t="s">
         <v>19</v>
       </c>
@@ -1575,19 +1617,19 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B61" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
-      <c r="F61" s="7"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="6"/>
+      <c r="A62" s="7"/>
       <c r="B62" t="s">
         <v>12</v>
       </c>
@@ -2053,11 +2095,1457 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6269139B-0747-4370-9E90-0B08ADC8D579}">
+  <dimension ref="A1:K92"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="G84" sqref="G84"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>29</v>
+      </c>
+      <c r="H3">
+        <v>28</v>
+      </c>
+      <c r="I3">
+        <f>SUM(C3:H3)</f>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <f>1/6*132</f>
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:H4" si="0">1/6*132</f>
+        <v>22</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5">
+        <f>(C3-C4)^2/C4</f>
+        <v>1.6363636363636365</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:H5" si="1">(D3-D4)^2/D4</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>2.9090909090909092</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>2.2272727272727271</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>1.6363636363636365</v>
+      </c>
+      <c r="I5">
+        <f>SUM(C5:H5)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>9</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>8</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <f>SUM(C8:J8)</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:J10" si="2">(C8-C9)^2/C9</f>
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="K10">
+        <f>SUM(C10:J10)</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13">
+        <v>84</v>
+      </c>
+      <c r="D13">
+        <v>79</v>
+      </c>
+      <c r="E13">
+        <v>75</v>
+      </c>
+      <c r="F13">
+        <v>49</v>
+      </c>
+      <c r="G13">
+        <v>36</v>
+      </c>
+      <c r="H13">
+        <v>47</v>
+      </c>
+      <c r="I13">
+        <f>SUM(C13:H13)</f>
+        <v>370</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14">
+        <v>0.3</v>
+      </c>
+      <c r="D14">
+        <v>0.2</v>
+      </c>
+      <c r="E14">
+        <v>0.2</v>
+      </c>
+      <c r="F14">
+        <v>0.1</v>
+      </c>
+      <c r="G14">
+        <v>0.1</v>
+      </c>
+      <c r="H14">
+        <v>0.1</v>
+      </c>
+      <c r="I14">
+        <f>SUM(C14:H14)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <f>C14*370</f>
+        <v>111</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D15:H15" si="3">D14*370</f>
+        <v>74</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>74</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16">
+        <f>(C13-C15)^2/C15</f>
+        <v>6.5675675675675675</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:H16" si="4">(D13-D15)^2/D15</f>
+        <v>0.33783783783783783</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="4"/>
+        <v>1.3513513513513514E-2</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="4"/>
+        <v>3.8918918918918921</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="4"/>
+        <v>2.7027027027027029E-2</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="4"/>
+        <v>2.7027027027027026</v>
+      </c>
+      <c r="I16">
+        <f>SUM(C16:H16)</f>
+        <v>13.54054054054054</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19">
+        <v>24</v>
+      </c>
+      <c r="D19">
+        <v>37</v>
+      </c>
+      <c r="E19">
+        <v>39</v>
+      </c>
+      <c r="F19">
+        <f>SUM(C19:E19)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20">
+        <v>0.3</v>
+      </c>
+      <c r="D20">
+        <v>0.4</v>
+      </c>
+      <c r="E20">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21">
+        <f>C20*F19</f>
+        <v>30</v>
+      </c>
+      <c r="D21">
+        <v>40</v>
+      </c>
+      <c r="E21">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22">
+        <f>(C19-C21)^2/C21</f>
+        <v>1.2</v>
+      </c>
+      <c r="D22">
+        <f t="shared" ref="D22:E22" si="5">(D19-D21)^2/D21</f>
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="5"/>
+        <v>2.7</v>
+      </c>
+      <c r="F22">
+        <f>SUM(C22:E22)</f>
+        <v>4.125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>23</v>
+      </c>
+      <c r="E27">
+        <v>39</v>
+      </c>
+      <c r="F27">
+        <v>19</v>
+      </c>
+      <c r="G27">
+        <v>14</v>
+      </c>
+      <c r="H27">
+        <f>SUM(C27:G27)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28">
+        <f>_xlfn.BINOM.DIST(C26,4,0.5,FALSE)</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="D28">
+        <f t="shared" ref="D28:G28" si="6">_xlfn.BINOM.DIST(D26,4,0.5,FALSE)</f>
+        <v>0.24999999999999994</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="6"/>
+        <v>0.375</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="6"/>
+        <v>0.25</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="6"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="H28">
+        <f>SUM(C28:G28)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29">
+        <f>C28*100</f>
+        <v>6.25</v>
+      </c>
+      <c r="D29">
+        <f t="shared" ref="D29:G29" si="7">D28*100</f>
+        <v>24.999999999999993</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="7"/>
+        <v>37.5</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="7"/>
+        <v>25</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="7"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30">
+        <f>(C27-C29)^2/C29</f>
+        <v>0.25</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ref="D30:G30" si="8">(D27-D29)^2/D29</f>
+        <v>0.15999999999999892</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="8"/>
+        <v>0.06</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="8"/>
+        <v>1.44</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="8"/>
+        <v>9.61</v>
+      </c>
+      <c r="H30">
+        <f>SUM(C30:G30)</f>
+        <v>11.519999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="7"/>
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>154</v>
+      </c>
+      <c r="D34">
+        <v>171</v>
+      </c>
+      <c r="E34">
+        <v>275</v>
+      </c>
+      <c r="G34">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35">
+        <f>C40*G34/G40</f>
+        <v>150</v>
+      </c>
+      <c r="D35">
+        <f>D40*600/1000</f>
+        <v>150</v>
+      </c>
+      <c r="E35">
+        <f>E40*600/1000</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36">
+        <f>(C34-C35)^2/C35</f>
+        <v>0.10666666666666667</v>
+      </c>
+      <c r="D36">
+        <f t="shared" ref="D36:E36" si="9">(D34-D35)^2/D38</f>
+        <v>4.41</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="9"/>
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37">
+        <v>96</v>
+      </c>
+      <c r="D37">
+        <v>79</v>
+      </c>
+      <c r="E37">
+        <v>225</v>
+      </c>
+      <c r="G37">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38">
+        <f>G37*C40/G40</f>
+        <v>100</v>
+      </c>
+      <c r="D38">
+        <f>D40*400/1000</f>
+        <v>100</v>
+      </c>
+      <c r="E38">
+        <f>E40*400/1000</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39">
+        <f>(C37-C38)^2/C38</f>
+        <v>0.16</v>
+      </c>
+      <c r="D39">
+        <f t="shared" ref="D39:E39" si="10">(D37-D38)^2/D38</f>
+        <v>4.41</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="10"/>
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40">
+        <v>250</v>
+      </c>
+      <c r="D40">
+        <v>250</v>
+      </c>
+      <c r="E40">
+        <v>500</v>
+      </c>
+      <c r="G40">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42">
+        <f>SUM(C36:E36)+SUM(C39:E39)</f>
+        <v>15.336666666666666</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="6"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="7"/>
+      <c r="C45" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" t="s">
+        <v>21</v>
+      </c>
+      <c r="F45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46">
+        <v>22</v>
+      </c>
+      <c r="D46">
+        <v>74</v>
+      </c>
+      <c r="E46">
+        <v>102</v>
+      </c>
+      <c r="F46">
+        <f>SUM(C46:E46)</f>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47">
+        <f>C55*198/600</f>
+        <v>19.8</v>
+      </c>
+      <c r="D47">
+        <f t="shared" ref="D47:E47" si="11">D55*198/600</f>
+        <v>79.2</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="11"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48">
+        <f>(C46-C47)^2/C47</f>
+        <v>0.2444444444444443</v>
+      </c>
+      <c r="D48">
+        <f t="shared" ref="D48:E48" si="12">(D46-D47)^2/D47</f>
+        <v>0.34141414141414178</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="12"/>
+        <v>9.0909090909090912E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49">
+        <v>31</v>
+      </c>
+      <c r="D49">
+        <v>102</v>
+      </c>
+      <c r="E49">
+        <v>143</v>
+      </c>
+      <c r="F49">
+        <f t="shared" ref="F49:F52" si="13">SUM(C49:E49)</f>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>30</v>
+      </c>
+      <c r="C50">
+        <f>C55*276/600</f>
+        <v>27.6</v>
+      </c>
+      <c r="D50">
+        <f t="shared" ref="D50:E50" si="14">D55*276/600</f>
+        <v>110.4</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="14"/>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <f>(C49-C50)^2/C50</f>
+        <v>0.41884057971014454</v>
+      </c>
+      <c r="D51">
+        <f t="shared" ref="D51" si="15">(D49-D50)^2/D50</f>
+        <v>0.63913043478260956</v>
+      </c>
+      <c r="E51">
+        <f t="shared" ref="E51" si="16">(E49-E50)^2/E50</f>
+        <v>0.18115942028985507</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>79</v>
+      </c>
+      <c r="C52">
+        <v>7</v>
+      </c>
+      <c r="D52">
+        <v>64</v>
+      </c>
+      <c r="E52">
+        <v>55</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="13"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>30</v>
+      </c>
+      <c r="C53">
+        <f>C55*126/600</f>
+        <v>12.6</v>
+      </c>
+      <c r="D53">
+        <f t="shared" ref="D53:E53" si="17">D55*126/600</f>
+        <v>50.4</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="17"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <f>(C52-C53)^2/C53</f>
+        <v>2.4888888888888885</v>
+      </c>
+      <c r="D54">
+        <f t="shared" ref="D54" si="18">(D52-D53)^2/D53</f>
+        <v>3.6698412698412706</v>
+      </c>
+      <c r="E54">
+        <f t="shared" ref="E54" si="19">(E52-E53)^2/E53</f>
+        <v>1.0158730158730158</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55">
+        <v>60</v>
+      </c>
+      <c r="D55">
+        <v>240</v>
+      </c>
+      <c r="E55">
+        <v>300</v>
+      </c>
+      <c r="F55">
+        <f>SUM(C55:E55)</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>80</v>
+      </c>
+      <c r="C57">
+        <f>SUM(C48:E48)+SUM(C51:E51)+SUM(C54:E54)</f>
+        <v>9.0905012861534615</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="7"/>
+      <c r="C60" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" t="s">
+        <v>14</v>
+      </c>
+      <c r="F60" t="s">
+        <v>15</v>
+      </c>
+      <c r="G60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61">
+        <v>26</v>
+      </c>
+      <c r="D61">
+        <v>43</v>
+      </c>
+      <c r="E61">
+        <v>62</v>
+      </c>
+      <c r="F61">
+        <v>11</v>
+      </c>
+      <c r="G61">
+        <f>SUM(C61:F61)</f>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>30</v>
+      </c>
+      <c r="C62">
+        <f>C70*142/360</f>
+        <v>27.611111111111111</v>
+      </c>
+      <c r="D62">
+        <f t="shared" ref="D62:F62" si="20">D70*142/360</f>
+        <v>39.444444444444443</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="20"/>
+        <v>55.222222222222221</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="20"/>
+        <v>19.722222222222221</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>31</v>
+      </c>
+      <c r="C63">
+        <f>(C61-C62)^2/C62</f>
+        <v>9.4008495416946086E-2</v>
+      </c>
+      <c r="D63">
+        <f t="shared" ref="D63:F63" si="21">(D61-D62)^2/D62</f>
+        <v>0.32050078247261377</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="21"/>
+        <v>0.83188016990833913</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="21"/>
+        <v>3.8574334898278555</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>28</v>
+      </c>
+      <c r="C64">
+        <v>28</v>
+      </c>
+      <c r="D64">
+        <v>40</v>
+      </c>
+      <c r="E64">
+        <v>59</v>
+      </c>
+      <c r="F64">
+        <v>20</v>
+      </c>
+      <c r="G64">
+        <f t="shared" ref="G64:G67" si="22">SUM(C64:F64)</f>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>30</v>
+      </c>
+      <c r="C65">
+        <f>C70*147/360</f>
+        <v>28.583333333333332</v>
+      </c>
+      <c r="D65">
+        <f t="shared" ref="D65:F65" si="23">D70*147/360</f>
+        <v>40.833333333333336</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="23"/>
+        <v>57.166666666666664</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="23"/>
+        <v>20.416666666666668</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>31</v>
+      </c>
+      <c r="C66">
+        <f>(C64-C65)^2/C65</f>
+        <v>1.1904761904761857E-2</v>
+      </c>
+      <c r="D66">
+        <f t="shared" ref="D66" si="24">(D64-D65)^2/D65</f>
+        <v>1.7006802721088531E-2</v>
+      </c>
+      <c r="E66">
+        <f t="shared" ref="E66" si="25">(E64-E65)^2/E65</f>
+        <v>5.8794946550048743E-2</v>
+      </c>
+      <c r="F66">
+        <f t="shared" ref="F66" si="26">(F64-F65)^2/F65</f>
+        <v>8.5034013605442653E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67">
+        <v>16</v>
+      </c>
+      <c r="D67">
+        <v>17</v>
+      </c>
+      <c r="E67">
+        <v>19</v>
+      </c>
+      <c r="F67">
+        <v>19</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="22"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>30</v>
+      </c>
+      <c r="C68">
+        <f>C70*71/360</f>
+        <v>13.805555555555555</v>
+      </c>
+      <c r="D68">
+        <f t="shared" ref="D68:F68" si="27">D70*71/360</f>
+        <v>19.722222222222221</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="27"/>
+        <v>27.611111111111111</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="27"/>
+        <v>9.8611111111111107</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>31</v>
+      </c>
+      <c r="C69">
+        <f>(C67-C68)^2/C68</f>
+        <v>0.34881511289961997</v>
+      </c>
+      <c r="D69">
+        <f t="shared" ref="D69" si="28">(D67-D68)^2/D68</f>
+        <v>0.37574334898278539</v>
+      </c>
+      <c r="E69">
+        <f t="shared" ref="E69" si="29">(E67-E68)^2/E68</f>
+        <v>2.6855577911915938</v>
+      </c>
+      <c r="F69">
+        <f t="shared" ref="F69" si="30">(F67-F68)^2/F68</f>
+        <v>8.4695618153364638</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <f>SUM(C67+C64+C61)</f>
+        <v>70</v>
+      </c>
+      <c r="D70">
+        <f t="shared" ref="D70:E70" si="31">SUM(D67+D64+D61)</f>
+        <v>100</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="31"/>
+        <v>140</v>
+      </c>
+      <c r="F70">
+        <f>SUM(F67+F64+F61)</f>
+        <v>50</v>
+      </c>
+      <c r="G70">
+        <f>SUM(C70:F70)</f>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>80</v>
+      </c>
+      <c r="C72">
+        <f>SUM(C63:F63)+SUM(C66:F66)+SUM(C69:F69)</f>
+        <v>17.079710918572662</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>33</v>
+      </c>
+      <c r="B75" t="s">
+        <v>72</v>
+      </c>
+      <c r="C75" t="s">
+        <v>35</v>
+      </c>
+      <c r="D75" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>29</v>
+      </c>
+      <c r="C76">
+        <f>1000-546</f>
+        <v>454</v>
+      </c>
+      <c r="D76">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>30</v>
+      </c>
+      <c r="C77">
+        <v>500</v>
+      </c>
+      <c r="D77">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>67</v>
+      </c>
+      <c r="C78">
+        <f>(ABS(C76-C77)-0.5)^2/C77</f>
+        <v>4.1405000000000003</v>
+      </c>
+      <c r="D78">
+        <f>(ABS(D76-D77)-0.5)^2/D77</f>
+        <v>4.1405000000000003</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>80</v>
+      </c>
+      <c r="C80">
+        <f>C78+D78</f>
+        <v>8.2810000000000006</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>40</v>
+      </c>
+      <c r="C82" t="s">
+        <v>74</v>
+      </c>
+      <c r="D82" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>42</v>
+      </c>
+      <c r="C84">
+        <v>75</v>
+      </c>
+      <c r="D84">
+        <v>65</v>
+      </c>
+      <c r="E84">
+        <f>SUM(C84:D84)</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>30</v>
+      </c>
+      <c r="C85">
+        <f>C90*140/200</f>
+        <v>70</v>
+      </c>
+      <c r="D85">
+        <f>D90*140/200</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>67</v>
+      </c>
+      <c r="C86">
+        <f>(ABS(C84-C85)-0.5)^2/C85</f>
+        <v>0.28928571428571431</v>
+      </c>
+      <c r="D86">
+        <f>(ABS(D84-D85)-0.5)^2/D85</f>
+        <v>0.28928571428571431</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>43</v>
+      </c>
+      <c r="C87">
+        <f>C90-C84</f>
+        <v>25</v>
+      </c>
+      <c r="D87">
+        <f>D90-D84</f>
+        <v>35</v>
+      </c>
+      <c r="E87">
+        <f>SUM(C87:D87)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>30</v>
+      </c>
+      <c r="C88">
+        <f>C90*60/E90</f>
+        <v>30</v>
+      </c>
+      <c r="D88">
+        <f>D90*60/200</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>67</v>
+      </c>
+      <c r="C89">
+        <f>(ABS(C87-C88)-0.5)^2/C88</f>
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="D89">
+        <f>(ABS(D87-D88)-0.5)^2/D88</f>
+        <v>0.67500000000000004</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>32</v>
+      </c>
+      <c r="C90">
+        <v>100</v>
+      </c>
+      <c r="D90">
+        <v>100</v>
+      </c>
+      <c r="E90">
+        <f>SUM(C90:D90)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>80</v>
+      </c>
+      <c r="C92">
+        <f>SUM(C86:D86)+SUM(C89:D89)</f>
+        <v>1.9285714285714288</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:G59"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA040C73-D898-4B5C-AE7A-712AD1E977BF}">
   <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2174,17 +3662,17 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
+      <c r="A9" s="7"/>
       <c r="B9" t="s">
         <v>19</v>
       </c>
@@ -2383,19 +3871,19 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
+      <c r="A25" s="7"/>
       <c r="B25" t="s">
         <v>12</v>
       </c>
@@ -2801,324 +4289,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6269139B-0747-4370-9E90-0B08ADC8D579}">
-  <dimension ref="A1:K13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:H13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3">
-        <v>16</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-      <c r="E3">
-        <v>25</v>
-      </c>
-      <c r="F3">
-        <v>14</v>
-      </c>
-      <c r="G3">
-        <v>29</v>
-      </c>
-      <c r="H3">
-        <v>28</v>
-      </c>
-      <c r="I3">
-        <f>SUM(C3:H3)</f>
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4">
-        <f>1/6*132</f>
-        <v>22</v>
-      </c>
-      <c r="D4">
-        <f t="shared" ref="D4:H4" si="0">1/6*132</f>
-        <v>22</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5">
-        <f>(C3-C4)^2/C4</f>
-        <v>1.6363636363636365</v>
-      </c>
-      <c r="D5">
-        <f t="shared" ref="D5:H5" si="1">(D3-D4)^2/D4</f>
-        <v>0.18181818181818182</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="1"/>
-        <v>0.40909090909090912</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="1"/>
-        <v>2.9090909090909092</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="1"/>
-        <v>2.2272727272727271</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="1"/>
-        <v>1.6363636363636365</v>
-      </c>
-      <c r="I5">
-        <f>SUM(C5:H5)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <v>4</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7">
-        <v>6</v>
-      </c>
-      <c r="I7">
-        <v>7</v>
-      </c>
-      <c r="J7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8">
-        <v>8</v>
-      </c>
-      <c r="D8">
-        <v>7</v>
-      </c>
-      <c r="E8">
-        <v>6</v>
-      </c>
-      <c r="F8">
-        <v>9</v>
-      </c>
-      <c r="G8">
-        <v>10</v>
-      </c>
-      <c r="H8">
-        <v>8</v>
-      </c>
-      <c r="I8">
-        <v>6</v>
-      </c>
-      <c r="J8">
-        <v>10</v>
-      </c>
-      <c r="K8">
-        <f>SUM(C8:J8)</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
-      </c>
-      <c r="D9">
-        <v>8</v>
-      </c>
-      <c r="E9">
-        <v>8</v>
-      </c>
-      <c r="F9">
-        <v>8</v>
-      </c>
-      <c r="G9">
-        <v>8</v>
-      </c>
-      <c r="H9">
-        <v>8</v>
-      </c>
-      <c r="I9">
-        <v>8</v>
-      </c>
-      <c r="J9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10">
-        <f>(C8-C9)^2/C9</f>
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <f t="shared" ref="D10:J10" si="2">(D8-D9)^2/D9</f>
-        <v>0.125</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="2"/>
-        <v>0.125</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="K10">
-        <f>SUM(C10:J10)</f>
-        <v>2.25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" t="s">
-        <v>57</v>
-      </c>
-      <c r="H12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13">
-        <v>84</v>
-      </c>
-      <c r="D13">
-        <v>79</v>
-      </c>
-      <c r="E13">
-        <v>75</v>
-      </c>
-      <c r="F13">
-        <v>49</v>
-      </c>
-      <c r="G13">
-        <v>36</v>
-      </c>
-      <c r="H13">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>